<commit_message>
started to work on creating a Class for drawings, and loading data in so we can save it back to the workbooks.
</commit_message>
<xml_diff>
--- a/examples/drawings/in.xlsx
+++ b/examples/drawings/in.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -167,6 +169,116 @@
         <a:xfrm>
           <a:off x="8505824" y="2786743"/>
           <a:ext cx="4495801" cy="4476751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352984</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>175167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{950E4666-68F4-4D9A-9225-094B86DF2ACC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7058584" cy="1127667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219191</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66737</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04A2F339-DD91-44C6-BF00-8A5258B7318A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="828791" cy="447737"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -443,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
@@ -452,4 +564,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43734AFA-758F-43D6-A452-10D27306463E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41AAE8-EB1A-4839-9ED0-10DA8042D053}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a check to see if we need to load drawings or not per sheet
</commit_message>
<xml_diff>
--- a/examples/drawings/in.xlsx
+++ b/examples/drawings/in.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -583,11 +587,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41AAE8-EB1A-4839-9ED0-10DA8042D053}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA39C181-A2C7-47C4-84B0-9FB4A32300B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD7FFE4-B46A-4AA6-80DC-E0D9DB561DD3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E84984-5722-4269-A38A-0B7D892CDE89}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F126C37E-1AF1-4CD4-91B3-9BAABA1F0B85}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a comment, and also added in a better testing xlsx file. with everything in it that could break due to changing drawings.
</commit_message>
<xml_diff>
--- a/examples/drawings/in.xlsx
+++ b/examples/drawings/in.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -136,6 +137,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-348F-48C2-8034-C310DA2A8411}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -151,6 +157,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-348F-48C2-8034-C310DA2A8411}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -166,6 +177,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-348F-48C2-8034-C310DA2A8411}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -181,6 +197,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-348F-48C2-8034-C310DA2A8411}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -317,7 +338,361 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5048556430446214E-2"/>
+          <c:y val="5.0925925925925923E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2692038495188102E-2"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.89653018372703408"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$I$6:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA8A-4CA5-A667-ED38F502D3B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="426680536"/>
+        <c:axId val="426681192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="426680536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426681192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="426681192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426680536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -876,6 +1251,3996 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="accent1" pri="11200"/>
+  </dgm:catLst>
+  <dgm:styleLbl name="node0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="dk1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+</dgm:colorsDef>
+</file>
+
+<file path=xl/diagrams/data1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dgm:ptLst>
+    <dgm:pt modelId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" type="doc">
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/list1" loCatId="list" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B341D079-C8B9-465D-8CE4-55B47FBC4985}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2BE72D75-A1BB-4FA2-ABD1-AE522B53255C}" type="parTrans" cxnId="{6A864054-C41A-475F-9520-E0B9BBF4FD00}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{ED4A9751-A760-4915-93A1-28482DC1C0A7}" type="sibTrans" cxnId="{6A864054-C41A-475F-9520-E0B9BBF4FD00}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}">
+      <dgm:prSet phldrT="[Text]" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2B82F520-E5DF-4129-8FAB-167BD38F964A}" type="parTrans" cxnId="{90769747-3096-4028-B1E7-77921B36E8B5}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0E9B9A81-EFF0-4F34-9250-503A5BC11F3E}" type="sibTrans" cxnId="{90769747-3096-4028-B1E7-77921B36E8B5}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}">
+      <dgm:prSet phldrT="[Text]" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{43BC33A9-B742-4891-9DA9-1C88745F69D7}" type="parTrans" cxnId="{C81563B0-946F-4F15-8CAB-64EFE3D0C4D8}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{EF5E7D09-7F30-4D9D-86BC-8783D411CDE9}" type="sibTrans" cxnId="{C81563B0-946F-4F15-8CAB-64EFE3D0C4D8}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{35E11B40-E447-42B1-A0EB-837DC6708C3E}" type="parTrans" cxnId="{223F2457-1B34-4DD2-AB28-FAF636EF62A1}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{766A80E0-DA56-4AED-91C0-3C8B91CC7E97}" type="sibTrans" cxnId="{223F2457-1B34-4DD2-AB28-FAF636EF62A1}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A4440CBD-1103-42B9-B54A-8150864EEF5B}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F5FC9D38-C833-43D6-A0EC-BC674BA7778E}" type="parTrans" cxnId="{689F8EF6-A057-48C8-BC14-8DD3825D06F5}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F72B476F-B8E4-4A44-A018-C09F290BC7AB}" type="sibTrans" cxnId="{689F8EF6-A057-48C8-BC14-8DD3825D06F5}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{752E69A0-4488-4764-A474-591F1E4942FB}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{04FBA362-C17F-499A-AD6A-06D27CD3FE69}" type="parTrans" cxnId="{BBABC67F-EC11-4E5C-B048-E6FF9EC95388}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{ABBC2F41-938E-4F17-B3FE-44A17F1485C4}" type="sibTrans" cxnId="{BBABC67F-EC11-4E5C-B048-E6FF9EC95388}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>`</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CC1611B3-553B-49DB-A209-6327D74FC8A5}" type="parTrans" cxnId="{585CC25F-B888-4C9F-A697-341CDA278CAD}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2A5E05F7-8ADD-4D86-ACE9-461FBC3733C7}" type="sibTrans" cxnId="{585CC25F-B888-4C9F-A697-341CDA278CAD}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" type="pres">
+      <dgm:prSet presAssocID="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" presName="linear" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:dir/>
+          <dgm:animLvl val="lvl"/>
+          <dgm:resizeHandles val="exact"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{397CEDBB-5D1E-4732-BD03-7CB219F0C3B0}" type="pres">
+      <dgm:prSet presAssocID="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{BCDB5E31-EC17-4325-AAFE-E4A48C32B921}" type="pres">
+      <dgm:prSet presAssocID="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{DB3EE330-FD77-47FE-8F3C-5EE2706DA9E3}" type="pres">
+      <dgm:prSet presAssocID="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" presName="parentText" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FE5BA1BF-2574-4392-9F30-EB02F5977989}" type="pres">
+      <dgm:prSet presAssocID="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B123BC98-A153-44BA-B9FF-970DB3FFF979}" type="pres">
+      <dgm:prSet presAssocID="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="0" presStyleCnt="7" custLinFactY="100000" custLinFactNeighborX="31667" custLinFactNeighborY="106597">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A453A135-80E2-4DC0-8B19-37F5D9DC64CB}" type="pres">
+      <dgm:prSet presAssocID="{ED4A9751-A760-4915-93A1-28482DC1C0A7}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C4323337-B8B1-44B6-941B-3ADC781DE31C}" type="pres">
+      <dgm:prSet presAssocID="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D06EB772-4B6E-4580-9BFF-F7015F0D6A35}" type="pres">
+      <dgm:prSet presAssocID="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{61E12294-CD97-471A-B464-702BB5821835}" type="pres">
+      <dgm:prSet presAssocID="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" presName="parentText" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{96BF203E-6187-471A-8183-365455DAE4FE}" type="pres">
+      <dgm:prSet presAssocID="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{55CCD26D-7B5E-49CD-96D3-E462A4FBC595}" type="pres">
+      <dgm:prSet presAssocID="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="1" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{818A7AA5-C54D-48B2-AE4E-EB966CC59896}" type="pres">
+      <dgm:prSet presAssocID="{766A80E0-DA56-4AED-91C0-3C8B91CC7E97}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{13BFF5A5-D5EC-4964-A5DC-32E2D14D6ACE}" type="pres">
+      <dgm:prSet presAssocID="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EC287893-AC6C-48A3-A9B0-F887B7B43836}" type="pres">
+      <dgm:prSet presAssocID="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2C08180E-03A1-4B8F-8E0A-4990C98D7E99}" type="pres">
+      <dgm:prSet presAssocID="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" presName="parentText" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{853B830E-02B8-440B-85CA-D74B9B5168F4}" type="pres">
+      <dgm:prSet presAssocID="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6A0D97CA-A0CF-4321-90EA-8BABCFC655A9}" type="pres">
+      <dgm:prSet presAssocID="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="2" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0B60E728-E010-44B3-A2BB-79ECF090EACD}" type="pres">
+      <dgm:prSet presAssocID="{F72B476F-B8E4-4A44-A018-C09F290BC7AB}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9F8D1074-A387-43DD-9117-BF91E45B3FFC}" type="pres">
+      <dgm:prSet presAssocID="{752E69A0-4488-4764-A474-591F1E4942FB}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E334B5BD-F2EB-4D43-8EBB-AD17E34182D8}" type="pres">
+      <dgm:prSet presAssocID="{752E69A0-4488-4764-A474-591F1E4942FB}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E379A7B2-4BC1-4C69-85BE-11A53C658D68}" type="pres">
+      <dgm:prSet presAssocID="{752E69A0-4488-4764-A474-591F1E4942FB}" presName="parentText" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C810414E-A431-4D05-ADB3-551AAC4F46C5}" type="pres">
+      <dgm:prSet presAssocID="{752E69A0-4488-4764-A474-591F1E4942FB}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6789BB77-AF32-4200-AC39-C2E496090804}" type="pres">
+      <dgm:prSet presAssocID="{752E69A0-4488-4764-A474-591F1E4942FB}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="3" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{66382D61-571F-4B0E-B58C-B609E2C01359}" type="pres">
+      <dgm:prSet presAssocID="{ABBC2F41-938E-4F17-B3FE-44A17F1485C4}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{54DD99DD-6B52-451E-BB5C-A8097B5153E8}" type="pres">
+      <dgm:prSet presAssocID="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A7DCD826-10F5-4962-9889-8541500F54A1}" type="pres">
+      <dgm:prSet presAssocID="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5AD08036-331E-4054-9BDD-2DA33274D238}" type="pres">
+      <dgm:prSet presAssocID="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" presName="parentText" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C37A7D29-BDFA-4787-9567-7FA0C5B7BC0C}" type="pres">
+      <dgm:prSet presAssocID="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1B49F3CE-5E06-4970-9600-2440A67AED57}" type="pres">
+      <dgm:prSet presAssocID="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="4" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{82387FD4-0271-4224-910C-96166AA0F474}" type="pres">
+      <dgm:prSet presAssocID="{2A5E05F7-8ADD-4D86-ACE9-461FBC3733C7}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A9D48480-F115-46A5-9CD8-3665304C5753}" type="pres">
+      <dgm:prSet presAssocID="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F5648BEA-E4B2-453B-8813-9FA7B89EF4C5}" type="pres">
+      <dgm:prSet presAssocID="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D8D46871-235E-483E-8201-EBAB8C504925}" type="pres">
+      <dgm:prSet presAssocID="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" presName="parentText" presStyleLbl="node1" presStyleIdx="5" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{29C1EB0A-5043-4E0D-B5FC-DF54E1B4FBE6}" type="pres">
+      <dgm:prSet presAssocID="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{53D64FCA-B35E-4E4A-8CB5-CD9402967467}" type="pres">
+      <dgm:prSet presAssocID="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="5" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EB5504B1-FAA8-4C60-8691-9942D2DC4AA0}" type="pres">
+      <dgm:prSet presAssocID="{0E9B9A81-EFF0-4F34-9250-503A5BC11F3E}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5A6893A1-8A1D-4D63-B6D6-BCE05BC6302B}" type="pres">
+      <dgm:prSet presAssocID="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" presName="parentLin" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E1CB2BA8-A19C-4437-8912-EAD8F4D3CFE8}" type="pres">
+      <dgm:prSet presAssocID="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="5" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{28077ADE-2FD2-47EF-AF46-3F1E3DA59FD4}" type="pres">
+      <dgm:prSet presAssocID="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" presName="parentText" presStyleLbl="node1" presStyleIdx="6" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="0"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8AD4565F-CF8A-49D3-8D75-1FA57802BB45}" type="pres">
+      <dgm:prSet presAssocID="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" presName="negativeSpace" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{4E10582F-38EE-4B80-93A2-8073198B32C3}" type="pres">
+      <dgm:prSet presAssocID="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" presName="childText" presStyleLbl="conFgAcc1" presStyleIdx="6" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+  </dgm:ptLst>
+  <dgm:cxnLst>
+    <dgm:cxn modelId="{1573BB5E-0D86-43CD-BF2D-CEBAAC7DC062}" type="presOf" srcId="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" destId="{A7DCD826-10F5-4962-9889-8541500F54A1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{585CC25F-B888-4C9F-A697-341CDA278CAD}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" srcOrd="4" destOrd="0" parTransId="{CC1611B3-553B-49DB-A209-6327D74FC8A5}" sibTransId="{2A5E05F7-8ADD-4D86-ACE9-461FBC3733C7}"/>
+    <dgm:cxn modelId="{0D259765-46C5-442C-9570-E0C5A98CCEF2}" type="presOf" srcId="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" destId="{28077ADE-2FD2-47EF-AF46-3F1E3DA59FD4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{90769747-3096-4028-B1E7-77921B36E8B5}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" srcOrd="5" destOrd="0" parTransId="{2B82F520-E5DF-4129-8FAB-167BD38F964A}" sibTransId="{0E9B9A81-EFF0-4F34-9250-503A5BC11F3E}"/>
+    <dgm:cxn modelId="{EF0ACA47-BDA4-458C-87E0-25AD1EC14461}" type="presOf" srcId="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" destId="{EC287893-AC6C-48A3-A9B0-F887B7B43836}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{6A864054-C41A-475F-9520-E0B9BBF4FD00}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" srcOrd="0" destOrd="0" parTransId="{2BE72D75-A1BB-4FA2-ABD1-AE522B53255C}" sibTransId="{ED4A9751-A760-4915-93A1-28482DC1C0A7}"/>
+    <dgm:cxn modelId="{AC5EFA75-7A8D-4E7C-A9F8-69CE1D79D667}" type="presOf" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{223F2457-1B34-4DD2-AB28-FAF636EF62A1}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" srcOrd="1" destOrd="0" parTransId="{35E11B40-E447-42B1-A0EB-837DC6708C3E}" sibTransId="{766A80E0-DA56-4AED-91C0-3C8B91CC7E97}"/>
+    <dgm:cxn modelId="{EF332E7F-4B94-46B6-A57A-CE157CBA0937}" type="presOf" srcId="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" destId="{61E12294-CD97-471A-B464-702BB5821835}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{BBABC67F-EC11-4E5C-B048-E6FF9EC95388}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{752E69A0-4488-4764-A474-591F1E4942FB}" srcOrd="3" destOrd="0" parTransId="{04FBA362-C17F-499A-AD6A-06D27CD3FE69}" sibTransId="{ABBC2F41-938E-4F17-B3FE-44A17F1485C4}"/>
+    <dgm:cxn modelId="{2038CA7F-B540-4C10-8818-2BA0AFDC1514}" type="presOf" srcId="{752E69A0-4488-4764-A474-591F1E4942FB}" destId="{E379A7B2-4BC1-4C69-85BE-11A53C658D68}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{01CC4D86-6CFF-421C-A0AD-AA29F6BCAF0A}" type="presOf" srcId="{88E24909-3129-4F1F-BAEA-B7ABA9C5CD50}" destId="{D06EB772-4B6E-4580-9BFF-F7015F0D6A35}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{71889086-7C83-41B8-8239-AEE44D8EEE84}" type="presOf" srcId="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" destId="{F5648BEA-E4B2-453B-8813-9FA7B89EF4C5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{67504191-6398-49CE-B50C-BA2C0D50B6A4}" type="presOf" srcId="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" destId="{BCDB5E31-EC17-4325-AAFE-E4A48C32B921}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{1B2CBC9B-565A-46B0-BAC9-BAAA2511A598}" type="presOf" srcId="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" destId="{2C08180E-03A1-4B8F-8E0A-4990C98D7E99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{5F0659A7-EAC7-4133-A0AD-2D7C1B78119C}" type="presOf" srcId="{896F82CE-F7AA-4D29-A5B1-6C5EC7CCD435}" destId="{5AD08036-331E-4054-9BDD-2DA33274D238}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{C81563B0-946F-4F15-8CAB-64EFE3D0C4D8}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" srcOrd="6" destOrd="0" parTransId="{43BC33A9-B742-4891-9DA9-1C88745F69D7}" sibTransId="{EF5E7D09-7F30-4D9D-86BC-8783D411CDE9}"/>
+    <dgm:cxn modelId="{2099A3C0-74CD-4726-BFDD-41A0E6D0279E}" type="presOf" srcId="{B341D079-C8B9-465D-8CE4-55B47FBC4985}" destId="{DB3EE330-FD77-47FE-8F3C-5EE2706DA9E3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{6303D4C5-071A-4D11-8075-A897113DFBCE}" type="presOf" srcId="{8FF795E4-1AF0-4AF9-BCAE-5D83EACA2E6E}" destId="{D8D46871-235E-483E-8201-EBAB8C504925}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{53904AD7-3A58-4191-89A7-A8ABA2C3BBFA}" type="presOf" srcId="{752E69A0-4488-4764-A474-591F1E4942FB}" destId="{E334B5BD-F2EB-4D43-8EBB-AD17E34182D8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{72E47FF6-E87B-4B48-B1F7-ADE426B0FC5C}" type="presOf" srcId="{727FFB12-1FBF-458C-A0FA-1835DF7852D1}" destId="{E1CB2BA8-A19C-4437-8912-EAD8F4D3CFE8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{689F8EF6-A057-48C8-BC14-8DD3825D06F5}" srcId="{FB0FF11D-56F4-49E4-B05E-FD38B98C4234}" destId="{A4440CBD-1103-42B9-B54A-8150864EEF5B}" srcOrd="2" destOrd="0" parTransId="{F5FC9D38-C833-43D6-A0EC-BC674BA7778E}" sibTransId="{F72B476F-B8E4-4A44-A018-C09F290BC7AB}"/>
+    <dgm:cxn modelId="{75E91FA2-1B59-4437-8F5A-6B269C4B8047}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{397CEDBB-5D1E-4732-BD03-7CB219F0C3B0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{4C40E58B-4686-472A-BDC6-BF2FD178E3B8}" type="presParOf" srcId="{397CEDBB-5D1E-4732-BD03-7CB219F0C3B0}" destId="{BCDB5E31-EC17-4325-AAFE-E4A48C32B921}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{9D4B20D8-23A5-4976-BB42-0B3684579A26}" type="presParOf" srcId="{397CEDBB-5D1E-4732-BD03-7CB219F0C3B0}" destId="{DB3EE330-FD77-47FE-8F3C-5EE2706DA9E3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{ACF725FA-F912-4BDE-AA37-AD6AF3371262}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{FE5BA1BF-2574-4392-9F30-EB02F5977989}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{F79BCE89-CF0F-47F4-8850-F81253A20F94}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{B123BC98-A153-44BA-B9FF-970DB3FFF979}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{1D367134-B0CB-4044-A62D-704998CC7845}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{A453A135-80E2-4DC0-8B19-37F5D9DC64CB}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{F2164F88-F9BD-4AD3-BEA2-61F58FABA534}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{C4323337-B8B1-44B6-941B-3ADC781DE31C}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{6C6DD07C-3D75-42E9-B23D-3F53099BD766}" type="presParOf" srcId="{C4323337-B8B1-44B6-941B-3ADC781DE31C}" destId="{D06EB772-4B6E-4580-9BFF-F7015F0D6A35}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{AB1B8825-7EC7-4E19-A6C0-824465D078F5}" type="presParOf" srcId="{C4323337-B8B1-44B6-941B-3ADC781DE31C}" destId="{61E12294-CD97-471A-B464-702BB5821835}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{E29CBB0A-5D39-4428-A626-E1406C99A166}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{96BF203E-6187-471A-8183-365455DAE4FE}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{83F5C202-BC7B-40F1-BA34-7E2A6E60D082}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{55CCD26D-7B5E-49CD-96D3-E462A4FBC595}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{9D988B1F-2958-4AF3-BBF7-C1A6C468D57A}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{818A7AA5-C54D-48B2-AE4E-EB966CC59896}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{91A7DF07-7B45-4B61-9895-F68F20ACF7F8}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{13BFF5A5-D5EC-4964-A5DC-32E2D14D6ACE}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{1439D005-20AA-4453-A8D1-D3051BD87A77}" type="presParOf" srcId="{13BFF5A5-D5EC-4964-A5DC-32E2D14D6ACE}" destId="{EC287893-AC6C-48A3-A9B0-F887B7B43836}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{B6D1F3FE-64DC-48C4-BA0F-E35D3F7D8E70}" type="presParOf" srcId="{13BFF5A5-D5EC-4964-A5DC-32E2D14D6ACE}" destId="{2C08180E-03A1-4B8F-8E0A-4990C98D7E99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{38ADB7DE-EE68-4AA6-BA16-F01D30331BD8}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{853B830E-02B8-440B-85CA-D74B9B5168F4}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{A8E69E87-E8E4-41E7-82EB-99D57BE7CC87}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{6A0D97CA-A0CF-4321-90EA-8BABCFC655A9}" srcOrd="10" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{617EAA71-C8FE-4EB0-82E4-69DA9A9A3429}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{0B60E728-E010-44B3-A2BB-79ECF090EACD}" srcOrd="11" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{853750D8-4E5D-49CA-B3A1-0DA9ACDE32CC}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{9F8D1074-A387-43DD-9117-BF91E45B3FFC}" srcOrd="12" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{DB64A718-F7C3-43B9-84D8-E60319F46047}" type="presParOf" srcId="{9F8D1074-A387-43DD-9117-BF91E45B3FFC}" destId="{E334B5BD-F2EB-4D43-8EBB-AD17E34182D8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{8EFF717C-5043-470D-A57B-05C5D3B3114F}" type="presParOf" srcId="{9F8D1074-A387-43DD-9117-BF91E45B3FFC}" destId="{E379A7B2-4BC1-4C69-85BE-11A53C658D68}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{AB59926A-136D-4CAE-A857-06AC33FCFFB0}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{C810414E-A431-4D05-ADB3-551AAC4F46C5}" srcOrd="13" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{215AD40F-521D-4F81-8A5F-24D2494B05A8}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{6789BB77-AF32-4200-AC39-C2E496090804}" srcOrd="14" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{7C19D8FF-EA5A-487C-A32A-2399410FCC3A}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{66382D61-571F-4B0E-B58C-B609E2C01359}" srcOrd="15" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{C6EAD4E5-9DC6-46A2-AD88-1B191711FA2A}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{54DD99DD-6B52-451E-BB5C-A8097B5153E8}" srcOrd="16" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{DFEC99C7-E424-4CD9-A226-8A7E7B63ACE4}" type="presParOf" srcId="{54DD99DD-6B52-451E-BB5C-A8097B5153E8}" destId="{A7DCD826-10F5-4962-9889-8541500F54A1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{10E05750-8168-4975-ADC5-0862F0C97131}" type="presParOf" srcId="{54DD99DD-6B52-451E-BB5C-A8097B5153E8}" destId="{5AD08036-331E-4054-9BDD-2DA33274D238}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{28795915-031B-4FA8-92C5-E1691809BB3D}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{C37A7D29-BDFA-4787-9567-7FA0C5B7BC0C}" srcOrd="17" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{83F5A450-4E67-46D1-803A-F2E55E87840E}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{1B49F3CE-5E06-4970-9600-2440A67AED57}" srcOrd="18" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{D54A7647-EF9A-4192-B1DE-0668E5F2D7FF}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{82387FD4-0271-4224-910C-96166AA0F474}" srcOrd="19" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{FF8734FB-787B-4E3E-BA3E-C113E2447863}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{A9D48480-F115-46A5-9CD8-3665304C5753}" srcOrd="20" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{55E2F2F7-6B5B-42A9-AE9A-F824612D08D0}" type="presParOf" srcId="{A9D48480-F115-46A5-9CD8-3665304C5753}" destId="{F5648BEA-E4B2-453B-8813-9FA7B89EF4C5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{9A1D3F56-6336-4B10-BB86-04FD89E0E886}" type="presParOf" srcId="{A9D48480-F115-46A5-9CD8-3665304C5753}" destId="{D8D46871-235E-483E-8201-EBAB8C504925}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{E382B9C9-8536-4132-8FA7-D1836B32FA3B}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{29C1EB0A-5043-4E0D-B5FC-DF54E1B4FBE6}" srcOrd="21" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{DF42C1BC-5960-4D80-B605-CC963C4372FA}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{53D64FCA-B35E-4E4A-8CB5-CD9402967467}" srcOrd="22" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{0F5C2878-9213-403C-A765-B2E929BF418B}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{EB5504B1-FAA8-4C60-8691-9942D2DC4AA0}" srcOrd="23" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{0C429D78-31A2-4F2E-BDC2-15C30322FCA3}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{5A6893A1-8A1D-4D63-B6D6-BCE05BC6302B}" srcOrd="24" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{045FCBF1-7DF1-4D2B-91B8-2D09AC343886}" type="presParOf" srcId="{5A6893A1-8A1D-4D63-B6D6-BCE05BC6302B}" destId="{E1CB2BA8-A19C-4437-8912-EAD8F4D3CFE8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{8D6CF4E6-15AB-43FD-A591-B1F23CF1D78D}" type="presParOf" srcId="{5A6893A1-8A1D-4D63-B6D6-BCE05BC6302B}" destId="{28077ADE-2FD2-47EF-AF46-3F1E3DA59FD4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{81752B39-F51E-4070-9BA5-2A9E72C8811C}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{8AD4565F-CF8A-49D3-8D75-1FA57802BB45}" srcOrd="25" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{F2AB6963-EC6F-43D4-AE54-D352C30EDCDB}" type="presParOf" srcId="{BFF5F016-C0B7-4920-A320-99EB6694E689}" destId="{4E10582F-38EE-4B80-93A2-8073198B32C3}" srcOrd="26" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+  </dgm:cxnLst>
+  <dgm:bg/>
+  <dgm:whole/>
+  <dgm:extLst>
+    <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
+      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId9" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+    </a:ext>
+  </dgm:extLst>
+</dgm:dataModel>
+</file>
+
+<file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dsp:spTree>
+    <dsp:nvGrpSpPr>
+      <dsp:cNvPr id="0" name=""/>
+      <dsp:cNvGrpSpPr/>
+    </dsp:nvGrpSpPr>
+    <dsp:grpSpPr/>
+    <dsp:sp modelId="{B123BC98-A153-44BA-B9FF-970DB3FFF979}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="488849"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{DB3EE330-FD77-47FE-8F3C-5EE2706DA9E3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="123120"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" kern="1200"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="134648"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{55CCD26D-7B5E-49CD-96D3-E462A4FBC595}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="604080"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{61E12294-CD97-471A-B464-702BB5821835}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="486000"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" kern="1200"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="497528"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{6A0D97CA-A0CF-4321-90EA-8BABCFC655A9}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="966960"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{2C08180E-03A1-4B8F-8E0A-4990C98D7E99}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="848880"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" kern="1200"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="860408"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{6789BB77-AF32-4200-AC39-C2E496090804}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1329840"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{E379A7B2-4BC1-4C69-85BE-11A53C658D68}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="1211759"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" kern="1200"/>
+            <a:t>asd</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="1223287"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{1B49F3CE-5E06-4970-9600-2440A67AED57}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1692720"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{5AD08036-331E-4054-9BDD-2DA33274D238}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="1574640"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="800" kern="1200"/>
+            <a:t>`</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="1586168"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{53D64FCA-B35E-4E4A-8CB5-CD9402967467}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2055600"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{D8D46871-235E-483E-8201-EBAB8C504925}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="1937520"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="800" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="1949048"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{4E10582F-38EE-4B80-93A2-8073198B32C3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2418480"/>
+          <a:ext cx="4572000" cy="201600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{28077ADE-2FD2-47EF-AF46-3F1E3DA59FD4}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="2300400"/>
+          <a:ext cx="3200400" cy="236160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="355600">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="800" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="240128" y="2311928"/>
+        <a:ext cx="3177344" cy="213104"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+  </dsp:spTree>
+</dsp:drawing>
+</file>
+
+<file path=xl/diagrams/layout1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:layoutDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/layout/list1">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="list" pri="4000"/>
+  </dgm:catLst>
+  <dgm:sampData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="2">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="3">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:sampData>
+  <dgm:styleData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="2"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:styleData>
+  <dgm:clrData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="3"/>
+        <dgm:pt modelId="4"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="5" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="7" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+        <dgm:cxn modelId="8" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:clrData>
+  <dgm:layoutNode name="linear">
+    <dgm:varLst>
+      <dgm:dir/>
+      <dgm:animLvl val="lvl"/>
+      <dgm:resizeHandles val="exact"/>
+    </dgm:varLst>
+    <dgm:choose name="Name0">
+      <dgm:if name="Name1" func="var" arg="dir" op="equ" val="norm">
+        <dgm:alg type="lin">
+          <dgm:param type="linDir" val="fromT"/>
+          <dgm:param type="vertAlign" val="mid"/>
+          <dgm:param type="horzAlign" val="l"/>
+          <dgm:param type="nodeHorzAlign" val="l"/>
+        </dgm:alg>
+      </dgm:if>
+      <dgm:else name="Name2">
+        <dgm:alg type="lin">
+          <dgm:param type="linDir" val="fromT"/>
+          <dgm:param type="vertAlign" val="mid"/>
+          <dgm:param type="horzAlign" val="r"/>
+          <dgm:param type="nodeHorzAlign" val="r"/>
+        </dgm:alg>
+      </dgm:else>
+    </dgm:choose>
+    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+      <dgm:adjLst/>
+    </dgm:shape>
+    <dgm:presOf/>
+    <dgm:constrLst>
+      <dgm:constr type="w" for="ch" forName="parentLin" refType="w"/>
+      <dgm:constr type="h" for="ch" forName="parentLin" val="INF"/>
+      <dgm:constr type="w" for="des" forName="parentLeftMargin" refType="w" fact="0.05"/>
+      <dgm:constr type="w" for="des" forName="parentText" refType="w" fact="0.7"/>
+      <dgm:constr type="h" for="des" forName="parentText" refType="primFontSz" refFor="des" refForName="parentText" fact="0.82"/>
+      <dgm:constr type="h" for="ch" forName="negativeSpace" refType="primFontSz" refFor="des" refForName="parentText" fact="-0.41"/>
+      <dgm:constr type="h" for="ch" forName="negativeSpace" refType="h" refFor="des" refForName="parentText" op="lte" fact="-0.82"/>
+      <dgm:constr type="h" for="ch" forName="negativeSpace" refType="h" refFor="des" refForName="parentText" op="gte" fact="-0.82"/>
+      <dgm:constr type="w" for="ch" forName="childText" refType="w"/>
+      <dgm:constr type="h" for="ch" forName="childText" refType="primFontSz" refFor="des" refForName="parentText" fact="0.7"/>
+      <dgm:constr type="primFontSz" for="des" forName="parentText" val="65"/>
+      <dgm:constr type="primFontSz" for="ch" forName="childText" refType="primFontSz" refFor="des" refForName="parentText"/>
+      <dgm:constr type="tMarg" for="ch" forName="childText" refType="primFontSz" refFor="des" refForName="parentText" fact="1.64"/>
+      <dgm:constr type="tMarg" for="ch" forName="childText" refType="h" refFor="des" refForName="parentText" op="lte" fact="3.28"/>
+      <dgm:constr type="tMarg" for="ch" forName="childText" refType="h" refFor="des" refForName="parentText" op="gte" fact="3.28"/>
+      <dgm:constr type="lMarg" for="ch" forName="childText" refType="w" fact="0.22"/>
+      <dgm:constr type="rMarg" for="ch" forName="childText" refType="lMarg" refFor="ch" refForName="childText"/>
+      <dgm:constr type="lMarg" for="des" forName="parentText" refType="w" fact="0.075"/>
+      <dgm:constr type="rMarg" for="des" forName="parentText" refType="lMarg" refFor="des" refForName="parentText"/>
+      <dgm:constr type="h" for="ch" forName="spaceBetweenRectangles" refType="primFontSz" refFor="des" refForName="parentText" fact="0.15"/>
+    </dgm:constrLst>
+    <dgm:ruleLst>
+      <dgm:rule type="primFontSz" for="des" forName="parentText" val="5" fact="NaN" max="NaN"/>
+    </dgm:ruleLst>
+    <dgm:forEach name="Name3" axis="ch" ptType="node">
+      <dgm:layoutNode name="parentLin">
+        <dgm:choose name="Name4">
+          <dgm:if name="Name5" func="var" arg="dir" op="equ" val="norm">
+            <dgm:alg type="lin">
+              <dgm:param type="linDir" val="fromL"/>
+              <dgm:param type="horzAlign" val="l"/>
+              <dgm:param type="nodeHorzAlign" val="l"/>
+            </dgm:alg>
+          </dgm:if>
+          <dgm:else name="Name6">
+            <dgm:alg type="lin">
+              <dgm:param type="linDir" val="fromR"/>
+              <dgm:param type="horzAlign" val="r"/>
+              <dgm:param type="nodeHorzAlign" val="r"/>
+            </dgm:alg>
+          </dgm:else>
+        </dgm:choose>
+        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+          <dgm:adjLst/>
+        </dgm:shape>
+        <dgm:presOf/>
+        <dgm:constrLst/>
+        <dgm:ruleLst/>
+        <dgm:layoutNode name="parentLeftMargin">
+          <dgm:alg type="sp"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="rect" r:blip="" hideGeom="1">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf axis="self"/>
+          <dgm:constrLst>
+            <dgm:constr type="h"/>
+          </dgm:constrLst>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+        <dgm:layoutNode name="parentText" styleLbl="node1">
+          <dgm:varLst>
+            <dgm:chMax val="0"/>
+            <dgm:bulletEnabled val="1"/>
+          </dgm:varLst>
+          <dgm:choose name="Name7">
+            <dgm:if name="Name8" func="var" arg="dir" op="equ" val="norm">
+              <dgm:alg type="tx">
+                <dgm:param type="parTxLTRAlign" val="l"/>
+                <dgm:param type="parTxRTLAlign" val="l"/>
+              </dgm:alg>
+            </dgm:if>
+            <dgm:else name="Name9">
+              <dgm:alg type="tx">
+                <dgm:param type="parTxLTRAlign" val="r"/>
+                <dgm:param type="parTxRTLAlign" val="r"/>
+              </dgm:alg>
+            </dgm:else>
+          </dgm:choose>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf axis="self" ptType="node"/>
+          <dgm:constrLst>
+            <dgm:constr type="tMarg"/>
+            <dgm:constr type="bMarg"/>
+          </dgm:constrLst>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+      </dgm:layoutNode>
+      <dgm:layoutNode name="negativeSpace">
+        <dgm:alg type="sp"/>
+        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+          <dgm:adjLst/>
+        </dgm:shape>
+        <dgm:presOf/>
+        <dgm:constrLst/>
+        <dgm:ruleLst/>
+      </dgm:layoutNode>
+      <dgm:layoutNode name="childText" styleLbl="conFgAcc1">
+        <dgm:varLst>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:varLst>
+        <dgm:alg type="tx">
+          <dgm:param type="stBulletLvl" val="1"/>
+        </dgm:alg>
+        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="rect" r:blip="" zOrderOff="-2">
+          <dgm:adjLst/>
+        </dgm:shape>
+        <dgm:presOf axis="des" ptType="node"/>
+        <dgm:constrLst>
+          <dgm:constr type="secFontSz" refType="primFontSz"/>
+        </dgm:constrLst>
+        <dgm:ruleLst>
+          <dgm:rule type="h" val="INF" fact="NaN" max="NaN"/>
+        </dgm:ruleLst>
+      </dgm:layoutNode>
+      <dgm:forEach name="Name10" axis="followSib" ptType="sibTrans" cnt="1">
+        <dgm:layoutNode name="spaceBetweenRectangles">
+          <dgm:alg type="sp"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf/>
+          <dgm:constrLst/>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+      </dgm:forEach>
+    </dgm:forEach>
+  </dgm:layoutNode>
+</dgm:layoutDef>
+</file>
+
+<file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="simple" pri="10100"/>
+  </dgm:catLst>
+  <dgm:scene3d>
+    <a:camera prst="orthographicFront"/>
+    <a:lightRig rig="threePt" dir="t"/>
+  </dgm:scene3d>
+  <dgm:styleLbl name="node0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="tx1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+</dgm:styleDef>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1029,6 +5394,246 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7061931D-3562-4886-B02B-CF72D36065C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1905000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55354211-F26F-4E53-B4CF-BC5E0F3C7CCF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2E24EE-F1A9-43FD-8E49-AC6B46FA89E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1895475" y="2495550"/>
+          <a:ext cx="2162175" cy="2524125"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Graphic 5" descr="Person with Cane">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCEBFB85-67DA-41E7-B876-04A41E694858}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="3619500"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagram 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09FB4F7F-D53E-4701-972B-9C8EF7D0E305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+          <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId5" r:lo="rId6" r:qs="rId7" r:cs="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1328,7 +5933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F0A158-D8FA-4404-AFCD-DD0D78DF83A0}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
@@ -1395,4 +6000,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33951F65-E42E-484E-B469-2A9BED125A87}">
+  <dimension ref="I6:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="6" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed drawing class loading in correct relationships, and also added more checks so it does not load anything other than an image into the class.
</commit_message>
<xml_diff>
--- a/examples/drawings/in.xlsx
+++ b/examples/drawings/in.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5920,7 +5920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EF672A-C984-4706-8709-9852ED56159F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -6006,7 +6006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33951F65-E42E-484E-B469-2A9BED125A87}">
   <dimension ref="I6:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>

</xml_diff>